<commit_message>
Moved folders so old version works again.
Also added some new material to subfolder; ok since using Rosebotics,
not the website, for the new stuff.
</commit_message>
<xml_diff>
--- a/plans/video_times_2015.xlsx
+++ b/plans/video_times_2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="11700" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>Unit</t>
   </si>
@@ -189,6 +189,51 @@
   </si>
   <si>
     <t>26:13</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>ActivitiesAndFragmentsOverview</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>CreatingActivity</t>
+  </si>
+  <si>
+    <t>UsingIntentExtras</t>
+  </si>
+  <si>
+    <t>UsingSystemIntents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IntroductionToFragments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backstack </t>
+  </si>
+  <si>
+    <t>LabComicViewer</t>
+  </si>
+  <si>
+    <t>ListFragment</t>
+  </si>
+  <si>
+    <t>DetailFragment</t>
+  </si>
+  <si>
+    <t>NavigationDrawer</t>
   </si>
 </sst>
 </file>
@@ -232,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -242,6 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,15 +592,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R39"/>
+  <dimension ref="A2:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32.7109375" customWidth="1"/>
   </cols>
@@ -644,6 +690,9 @@
       <c r="B17" s="2">
         <v>0.41250000000000003</v>
       </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -652,6 +701,9 @@
       <c r="B18" s="2">
         <v>0.33333333333333331</v>
       </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -660,6 +712,9 @@
       <c r="B19" s="2">
         <v>0.4513888888888889</v>
       </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -668,6 +723,9 @@
       <c r="B20" s="2">
         <v>0.32361111111111113</v>
       </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -676,6 +734,9 @@
       <c r="B21" s="2">
         <v>0.17152777777777775</v>
       </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -684,6 +745,9 @@
       <c r="B22" s="2">
         <v>0.75</v>
       </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -692,6 +756,9 @@
       <c r="B23" s="2">
         <v>0.57430555555555551</v>
       </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -700,6 +767,9 @@
       <c r="B24" s="2">
         <v>0.52777777777777779</v>
       </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -708,6 +778,9 @@
       <c r="B25" s="2">
         <v>9.2361111111111116E-2</v>
       </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -716,6 +789,9 @@
       <c r="B26" s="2">
         <v>0.5708333333333333</v>
       </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -724,6 +800,9 @@
       <c r="B27" s="2">
         <v>0.17708333333333334</v>
       </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -810,6 +889,78 @@
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.17916666666666667</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.17777777777777778</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="2">
+        <v>0.34166666666666662</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New plans for unit 4
</commit_message>
<xml_diff>
--- a/plans/video_times_2015.xlsx
+++ b/plans/video_times_2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="11700" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11700" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>Unit</t>
   </si>
@@ -234,6 +234,66 @@
   </si>
   <si>
     <t>NavigationDrawer</t>
+  </si>
+  <si>
+    <t>HistoricalDocsStartingCode</t>
+  </si>
+  <si>
+    <t>44 min</t>
+  </si>
+  <si>
+    <t>121 min</t>
+  </si>
+  <si>
+    <t>FirebaseOverview</t>
+  </si>
+  <si>
+    <t>WhatIsFirebase</t>
+  </si>
+  <si>
+    <t>SetupBackend</t>
+  </si>
+  <si>
+    <t>WebClient (optional)</t>
+  </si>
+  <si>
+    <t>SetupAndroid</t>
+  </si>
+  <si>
+    <t>PushingToFirebase</t>
+  </si>
+  <si>
+    <t>EventListeners</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>LabWeatherpics</t>
+  </si>
+  <si>
+    <t>83 min</t>
+  </si>
+  <si>
+    <t>94 min</t>
+  </si>
+  <si>
+    <t>72 min</t>
+  </si>
+  <si>
+    <t>45 min</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>10 videos</t>
+  </si>
+  <si>
+    <t>x min</t>
   </si>
 </sst>
 </file>
@@ -592,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R52"/>
+  <dimension ref="A2:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,354 +673,476 @@
         <v>26</v>
       </c>
     </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.3659722222222222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.6430555555555556</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.59513888888888888</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.21527777777777779</v>
+      </c>
+    </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2">
-        <v>0.3659722222222222</v>
+        <v>0.67361111111111116</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2">
-        <v>0.6430555555555556</v>
+        <v>0.77222222222222225</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2">
-        <v>0.59513888888888888</v>
-      </c>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.21527777777777779</v>
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.67361111111111116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.77222222222222225</v>
+      <c r="B11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2">
-        <v>0.17777777777777778</v>
-      </c>
-      <c r="R13" s="2"/>
+        <v>0.41250000000000003</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4">
-        <v>5.7638888888888885E-2</v>
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>44</v>
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.32361111111111113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2">
-        <v>0.41250000000000003</v>
+        <v>0.17152777777777775</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B18" s="2">
-        <v>0.33333333333333331</v>
+        <v>0.75</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2">
-        <v>0.4513888888888889</v>
+        <v>0.57430555555555551</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2">
-        <v>0.32361111111111113</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2">
-        <v>0.17152777777777775</v>
+        <v>9.2361111111111116E-2</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2">
-        <v>0.75</v>
+        <v>0.5708333333333333</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2">
-        <v>0.57430555555555551</v>
+        <v>0.17708333333333334</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="C24" t="s">
-        <v>60</v>
+      <c r="A24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="2">
-        <v>9.2361111111111116E-2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0.5708333333333333</v>
-      </c>
-      <c r="C26" t="s">
-        <v>61</v>
+      <c r="B25" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="2">
-        <v>0.17708333333333334</v>
-      </c>
-      <c r="C27" t="s">
-        <v>59</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="4">
-        <v>6.5277777777777782E-2</v>
-      </c>
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>43</v>
-      </c>
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.36458333333333331</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.17361111111111113</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="5"/>
+      <c r="A34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="2">
-        <v>0.36458333333333331</v>
+      <c r="B35" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B37" s="2">
-        <v>0.17361111111111113</v>
+        <v>0.17916666666666667</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="4">
-        <v>4.9999999999999996E-2</v>
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.17777777777777778</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>44</v>
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="2">
+        <v>0.34166666666666662</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.78888888888888886</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B41" s="2">
-        <v>0.17916666666666667</v>
+        <v>0.32013888888888892</v>
+      </c>
+      <c r="C41" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B42" s="2">
-        <v>0.17777777777777778</v>
+        <v>0.27361111111111108</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B43" s="2">
-        <v>0.34166666666666662</v>
+        <v>0.34791666666666665</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.59791666666666665</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="C45" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0.6791666666666667</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0.29236111111111113</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="B48" s="2">
+        <v>0.2673611111111111</v>
+      </c>
+      <c r="C48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B49" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0.16111111111111112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="2">
+        <v>8.4722222222222213E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="2">
+        <v>0.18611111111111112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unit 5 Firebase: deployed. Unit 4: couple tweaks.
Configuration file changed to point to firebase
</commit_message>
<xml_diff>
--- a/plans/video_times_2015.xlsx
+++ b/plans/video_times_2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="11700" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9240" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
   <si>
     <t>Unit</t>
   </si>
@@ -239,9 +239,6 @@
     <t>HistoricalDocsStartingCode</t>
   </si>
   <si>
-    <t>44 min</t>
-  </si>
-  <si>
     <t>121 min</t>
   </si>
   <si>
@@ -284,16 +281,58 @@
     <t>72 min</t>
   </si>
   <si>
-    <t>45 min</t>
-  </si>
-  <si>
-    <t>30 min</t>
-  </si>
-  <si>
     <t>10 videos</t>
   </si>
   <si>
     <t>x min</t>
+  </si>
+  <si>
+    <t>40 min, tight</t>
+  </si>
+  <si>
+    <t>37 min, tight</t>
+  </si>
+  <si>
+    <t>finish at home</t>
+  </si>
+  <si>
+    <t>in class, GOOD!</t>
+  </si>
+  <si>
+    <t>T/R</t>
+  </si>
+  <si>
+    <t>at home</t>
+  </si>
+  <si>
+    <t>32 min, OK</t>
+  </si>
+  <si>
+    <t>34 min, OK</t>
+  </si>
+  <si>
+    <t>37 min, right</t>
+  </si>
+  <si>
+    <t>took WAY too long. Need repo as backup, or some way to simplify. But I like having them create from scratch.</t>
+  </si>
+  <si>
+    <t>28 min, but need time to start ListFrag</t>
+  </si>
+  <si>
+    <t>33 min</t>
+  </si>
+  <si>
+    <t>at home, or Friday</t>
+  </si>
+  <si>
+    <t>31 min</t>
+  </si>
+  <si>
+    <t>Could add a day to do ValueEventListeners in the future!</t>
+  </si>
+  <si>
+    <t>34 min</t>
   </si>
 </sst>
 </file>
@@ -654,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,6 +719,9 @@
       <c r="B3" s="2">
         <v>0.3659722222222222</v>
       </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -688,6 +730,9 @@
       <c r="B4" s="2">
         <v>0.6430555555555556</v>
       </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -696,6 +741,12 @@
       <c r="B5" s="2">
         <v>0.59513888888888888</v>
       </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -704,6 +755,9 @@
       <c r="B6" s="2">
         <v>0.21527777777777779</v>
       </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -712,6 +766,9 @@
       <c r="B7" s="2">
         <v>0.67361111111111116</v>
       </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -720,6 +777,12 @@
       <c r="B8" s="2">
         <v>0.77222222222222225</v>
       </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -728,6 +791,9 @@
       <c r="B9" s="2">
         <v>0.17777777777777778</v>
       </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -735,7 +801,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -787,7 +853,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -797,8 +863,11 @@
       <c r="C17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -809,7 +878,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -820,7 +889,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -828,10 +897,10 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -839,10 +908,13 @@
         <v>9.2361111111111116E-2</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -852,8 +924,11 @@
       <c r="C22" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -864,161 +939,213 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="2">
         <v>0.36458333333333331</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="2">
         <v>0.17361111111111113</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>62</v>
       </c>
       <c r="B37" s="2">
         <v>0.17916666666666667</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
       <c r="B38" s="2">
         <v>0.17777777777777778</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>64</v>
       </c>
       <c r="B39" s="2">
         <v>0.34166666666666662</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>65</v>
       </c>
       <c r="B40" s="2">
         <v>0.78888888888888886</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>66</v>
       </c>
       <c r="B41" s="2">
         <v>0.32013888888888892</v>
       </c>
-      <c r="C41" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>72</v>
       </c>
       <c r="B42" s="2">
         <v>0.27361111111111108</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>73</v>
       </c>
       <c r="B43" s="2">
         <v>0.34791666666666665</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>67</v>
       </c>
       <c r="B44" s="2">
         <v>0.59791666666666665</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -1026,26 +1153,35 @@
         <v>0.71875</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>71</v>
       </c>
       <c r="B46" s="2">
         <v>0.6791666666666667</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>68</v>
       </c>
       <c r="B47" s="2">
         <v>0.29236111111111113</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>69</v>
       </c>
@@ -1053,7 +1189,7 @@
         <v>0.2673611111111111</v>
       </c>
       <c r="C48" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1061,7 +1197,7 @@
         <v>20</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1074,61 +1210,118 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52" s="2">
         <v>0.16111111111111112</v>
       </c>
+      <c r="C52" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53" s="2">
         <v>8.4722222222222213E-2</v>
       </c>
+      <c r="C53" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54" s="2">
         <v>0.18611111111111112</v>
       </c>
+      <c r="C54" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="B55" s="2">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="C55" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0.52916666666666667</v>
+      </c>
+      <c r="C56" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="B57" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="C57" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B58" s="2">
+        <v>0.53888888888888886</v>
+      </c>
+      <c r="C58" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="B59" s="2">
+        <v>0.21041666666666667</v>
+      </c>
+      <c r="C59" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="C60" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="C61" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1136,13 +1329,13 @@
         <v>20</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add materials for Firebase units 1 and 2
</commit_message>
<xml_diff>
--- a/plans/video_times_2015.xlsx
+++ b/plans/video_times_2015.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="121">
   <si>
     <t>Unit</t>
   </si>
@@ -284,9 +284,6 @@
     <t>10 videos</t>
   </si>
   <si>
-    <t>x min</t>
-  </si>
-  <si>
     <t>40 min, tight</t>
   </si>
   <si>
@@ -326,13 +323,61 @@
     <t>at home, or Friday</t>
   </si>
   <si>
-    <t>31 min</t>
-  </si>
-  <si>
     <t>Could add a day to do ValueEventListeners in the future!</t>
   </si>
   <si>
-    <t>34 min</t>
+    <t>74 min</t>
+  </si>
+  <si>
+    <t>FirebaseAuthenticationOverview</t>
+  </si>
+  <si>
+    <t>PasswordKeeper app</t>
+  </si>
+  <si>
+    <t>Rules</t>
+  </si>
+  <si>
+    <t>EmailPasswordAuthenticationSetup</t>
+  </si>
+  <si>
+    <t>EmailPasswordAuthenticationCode</t>
+  </si>
+  <si>
+    <t>GoogleAuthenticationSetup</t>
+  </si>
+  <si>
+    <t>GoogleAuthenticationCode</t>
+  </si>
+  <si>
+    <t>RoseFireAuthenticationSetup</t>
+  </si>
+  <si>
+    <t>RoseFireAuthenticationCode</t>
+  </si>
+  <si>
+    <t>LabOurWeatherpics</t>
+  </si>
+  <si>
+    <t>17 min, but long setup</t>
+  </si>
+  <si>
+    <t>22 min, relaxed, added true persistence offline</t>
+  </si>
+  <si>
+    <t>(do Bolt at end of class if time)</t>
+  </si>
+  <si>
+    <t>22 or 33</t>
+  </si>
+  <si>
+    <t>Do at home since SHA1 hash is painful.</t>
+  </si>
+  <si>
+    <t>Plus time for Tyler to explain the system</t>
+  </si>
+  <si>
+    <t>92 min</t>
   </si>
 </sst>
 </file>
@@ -691,15 +736,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R63"/>
+  <dimension ref="A2:R76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32.7109375" customWidth="1"/>
   </cols>
@@ -745,7 +790,7 @@
         <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -781,7 +826,7 @@
         <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -864,7 +909,7 @@
         <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,7 +942,7 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,7 +956,7 @@
         <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -925,7 +970,7 @@
         <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -996,7 +1041,7 @@
         <v>58</v>
       </c>
       <c r="D30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,7 +1066,7 @@
         <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1092,7 +1137,7 @@
         <v>58</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1103,7 +1148,7 @@
         <v>0.32013888888888892</v>
       </c>
       <c r="D41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1128,7 +1173,7 @@
         <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1142,7 +1187,7 @@
         <v>60</v>
       </c>
       <c r="D44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1167,7 +1212,7 @@
         <v>61</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,7 +1223,7 @@
         <v>0.29236111111111113</v>
       </c>
       <c r="D47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1251,6 +1296,9 @@
       <c r="C55" t="s">
         <v>58</v>
       </c>
+      <c r="D55" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -1260,10 +1308,7 @@
         <v>0.52916666666666667</v>
       </c>
       <c r="C56" t="s">
-        <v>58</v>
-      </c>
-      <c r="D56" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1287,6 +1332,9 @@
       <c r="C58" t="s">
         <v>60</v>
       </c>
+      <c r="D58" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -1296,7 +1344,7 @@
         <v>0.21041666666666667</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1307,21 +1355,21 @@
         <v>0.3833333333333333</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
-      </c>
-      <c r="D60" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>84</v>
       </c>
+      <c r="B61" s="2">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D61" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1329,12 +1377,126 @@
         <v>20</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C62" s="2"/>
+      <c r="D62" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>104</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0.22638888888888889</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" s="2">
+        <v>0.4368055555555555</v>
+      </c>
+      <c r="C67" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0.13263888888888889</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" s="2">
+        <v>0.5708333333333333</v>
+      </c>
+      <c r="C69">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>109</v>
+      </c>
+      <c r="B70" s="2">
+        <v>0.46319444444444446</v>
+      </c>
+      <c r="C70" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>110</v>
+      </c>
+      <c r="B71" s="2">
+        <v>0.9277777777777777</v>
+      </c>
+      <c r="C71" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>111</v>
+      </c>
+      <c r="B72" s="2">
+        <v>0.15833333333333333</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>112</v>
+      </c>
+      <c r="B73" s="2">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="C73">
+        <v>11</v>
+      </c>
+      <c r="D73" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>113</v>
+      </c>
+      <c r="B74" s="2">
+        <v>0.22916666666666666</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add materials for unit 7
</commit_message>
<xml_diff>
--- a/plans/video_times_2015.xlsx
+++ b/plans/video_times_2015.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9240" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="130">
   <si>
     <t>Unit</t>
   </si>
@@ -365,19 +365,46 @@
     <t>22 min, relaxed, added true persistence offline</t>
   </si>
   <si>
-    <t>(do Bolt at end of class if time)</t>
-  </si>
-  <si>
-    <t>22 or 33</t>
-  </si>
-  <si>
     <t>Do at home since SHA1 hash is painful.</t>
   </si>
   <si>
-    <t>Plus time for Tyler to explain the system</t>
-  </si>
-  <si>
     <t>92 min</t>
+  </si>
+  <si>
+    <t>FirebaseComplexDataOverview</t>
+  </si>
+  <si>
+    <t>FirebaseDataDesign</t>
+  </si>
+  <si>
+    <t>GradeRecorderSetup</t>
+  </si>
+  <si>
+    <t>GradeRecorderFirebaseCode</t>
+  </si>
+  <si>
+    <t>GradeRecorderFirebaseCodePart2</t>
+  </si>
+  <si>
+    <t>LabGradeRecorder</t>
+  </si>
+  <si>
+    <t>6 videos</t>
+  </si>
+  <si>
+    <t>I dilly-dallied and it went ~40 min. Glad they did setup at home.</t>
+  </si>
+  <si>
+    <t>Short class. Plenty of time for Tyler to explain the system.</t>
+  </si>
+  <si>
+    <t>(Skipped bolt)</t>
+  </si>
+  <si>
+    <t>21 then lab time.</t>
+  </si>
+  <si>
+    <t>65 min</t>
   </si>
 </sst>
 </file>
@@ -736,10 +763,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R76"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A2:R85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,6 +1424,9 @@
       <c r="B65" s="2">
         <v>0.22638888888888889</v>
       </c>
+      <c r="C65" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
@@ -1404,6 +1435,9 @@
       <c r="B66" s="2">
         <v>0.375</v>
       </c>
+      <c r="C66" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
@@ -1413,7 +1447,7 @@
         <v>0.4368055555555555</v>
       </c>
       <c r="C67" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1423,6 +1457,9 @@
       <c r="B68" s="2">
         <v>0.13263888888888889</v>
       </c>
+      <c r="C68" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -1431,7 +1468,10 @@
       <c r="B69" s="2">
         <v>0.5708333333333333</v>
       </c>
-      <c r="C69">
+      <c r="C69" t="s">
+        <v>58</v>
+      </c>
+      <c r="D69">
         <v>41</v>
       </c>
     </row>
@@ -1443,7 +1483,10 @@
         <v>0.46319444444444446</v>
       </c>
       <c r="C70" t="s">
-        <v>118</v>
+        <v>60</v>
+      </c>
+      <c r="D70" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1454,7 +1497,10 @@
         <v>0.9277777777777777</v>
       </c>
       <c r="C71" t="s">
-        <v>117</v>
+        <v>60</v>
+      </c>
+      <c r="D71" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1464,6 +1510,9 @@
       <c r="B72" s="2">
         <v>0.15833333333333333</v>
       </c>
+      <c r="C72" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -1472,11 +1521,11 @@
       <c r="B73" s="2">
         <v>0.30555555555555552</v>
       </c>
-      <c r="C73">
-        <v>11</v>
+      <c r="C73" t="s">
+        <v>61</v>
       </c>
       <c r="D73" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,18 +1535,106 @@
       <c r="B74" s="2">
         <v>0.22916666666666666</v>
       </c>
+      <c r="C74" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.20138888888888887</v>
+      </c>
+      <c r="C78" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>119</v>
+      </c>
+      <c r="B79" s="2">
+        <v>0.4694444444444445</v>
+      </c>
+      <c r="C79" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>120</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0.53680555555555554</v>
+      </c>
+      <c r="C80" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B81" s="2">
+        <v>0.65416666666666667</v>
+      </c>
+      <c r="C81" t="s">
+        <v>60</v>
+      </c>
+      <c r="D81">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>122</v>
+      </c>
+      <c r="B82" s="2">
+        <v>0.71319444444444446</v>
+      </c>
+      <c r="C82" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>123</v>
+      </c>
+      <c r="B83" s="2">
+        <v>0.15833333333333333</v>
+      </c>
+      <c r="C83" t="s">
+        <v>61</v>
+      </c>
+      <c r="D83" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1508,6 +1645,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>